<commit_message>
tests updated for changes
to admin file layout
</commit_message>
<xml_diff>
--- a/tests/samples/Hort.Res._Admin.xlsx
+++ b/tests/samples/Hort.Res._Admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC837BE-1927-4508-9CD6-2AD08D73E912}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27647284-F925-4176-AE46-FE3644F07A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22550" yWindow="4820" windowWidth="17690" windowHeight="15020" xr2:uid="{F7F7C31D-9B21-4E63-BF52-B7D512313953}"/>
+    <workbookView xWindow="31215" yWindow="1545" windowWidth="21600" windowHeight="11295" xr2:uid="{F7F7C31D-9B21-4E63-BF52-B7D512313953}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Client</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Save folder</t>
   </si>
   <si>
-    <t>auto select</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
   </si>
   <si>
     <t>&lt;!-- Specify whether to use the recorded times for each mass measurement in the least squares analysis of each circular weighing. Allowed options: YES or NO --&gt;</t>
-  </si>
-  <si>
-    <t>If relevant, include a matrix/list of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or matrix of correlations</t>
   </si>
   <si>
     <t>96240….</t>
@@ -247,12 +241,34 @@
   <si>
     <t>MSLT.M.001.008 Appendix D</t>
   </si>
+  <si>
+    <t>Config file</t>
+  </si>
+  <si>
+    <t>Expansion coeff (ppm/degC)</t>
+  </si>
+  <si>
+    <t>linear drift</t>
+  </si>
+  <si>
+    <t>If relevant, include a matrix/list of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or 2x2 matrix of correlations</t>
+  </si>
+  <si>
+    <t>Correct for air density?</t>
+  </si>
+  <si>
+    <t>If true, calculate basis 8000 mass differences using measured air density. Requires densities and expansion coefficients for all masses.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +319,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -333,10 +358,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -368,9 +394,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -404,9 +427,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{894EFE83-C161-4FCB-943A-D0359ABF64D9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,9 +458,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -462,7 +498,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -568,7 +604,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,7 +746,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,237 +754,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AB355D-84BE-43AB-B2BC-CDE069094A48}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:14" s="10" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C12" s="18"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="B13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="23"/>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <f>COUNT(B15:B69)</f>
         <v>9</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="F13" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+        <v>45</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <v>100</v>
       </c>
       <c r="B15" s="1">
@@ -959,9 +1020,10 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>50</v>
       </c>
       <c r="B16" s="1">
@@ -972,9 +1034,10 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>20</v>
       </c>
       <c r="B17" s="1">
@@ -985,24 +1048,26 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>37</v>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B18" s="1">
         <v>20</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="14">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>10</v>
       </c>
       <c r="B19" s="1">
@@ -1013,9 +1078,10 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="14">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>5</v>
       </c>
       <c r="B20" s="1">
@@ -1026,9 +1092,10 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>2</v>
       </c>
       <c r="B21" s="1">
@@ -1039,24 +1106,26 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>38</v>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="14">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>1</v>
       </c>
       <c r="B23" s="1">
@@ -1067,108 +1136,120 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="1"/>
       <c r="C24" s="7"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
       <c r="B25" s="1"/>
       <c r="C25" s="7"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="1"/>
       <c r="C26" s="7"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
       <c r="B27" s="1"/>
       <c r="C27" s="7"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
       <c r="B28" s="1"/>
       <c r="C28" s="7"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="1"/>
       <c r="C29" s="7"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="1"/>
       <c r="C30" s="7"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
       <c r="B31" s="1"/>
       <c r="C31" s="7"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="1"/>
       <c r="C32" s="7"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
       <c r="B33" s="1"/>
       <c r="C33" s="7"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="1"/>
       <c r="C34" s="7"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -1178,14 +1259,15 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="I7:N7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{A690A39A-7C4C-498C-8F5B-DEF5027274EF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{13DC46FE-8903-4E1E-8ACF-E8562A1A22A1}">
+      <formula1>"NO, YES"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{4B0743D5-C62A-4096-9A47-04ECFD934A79}">
       <formula1>"auto select, linear drift, quadratic drift, cubic drift"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{7969CC89-9911-42F9-96DF-8D0F0744D590}">
-      <formula1>"NO, YES"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>